<commit_message>
Added diagram for client state
</commit_message>
<xml_diff>
--- a/questions/Client Command Table A9.xlsx
+++ b/questions/Client Command Table A9.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyoun\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyoun\Desktop\CU_Boulder\ECEN5823\assignments\ecen5823_workspace\ecen5823-assignment9-hyounjunchang\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E0C93B-0BB3-4631-ABB7-C77271302A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11E9C6A-7113-4092-952C-5CC1435D4D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -720,6 +720,9 @@
     <xf numFmtId="49" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -731,9 +734,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,6 +818,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>96457</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>24113</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2624079</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>81942</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CA12639-4FD5-3471-ACAC-7403FB44905B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="96457" y="22269208"/>
+          <a:ext cx="7772400" cy="5796943"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1900,7 +1955,7 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -1918,13 +1973,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
@@ -2019,7 +2074,7 @@
       <c r="B9" s="4"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="44" t="s">
         <v>29</v>
       </c>
       <c r="F9" s="12" t="s">
@@ -2031,7 +2086,7 @@
       <c r="B10" s="4"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="43"/>
+      <c r="E10" s="44"/>
       <c r="F10" s="15" t="s">
         <v>14</v>
       </c>
@@ -2041,7 +2096,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="43"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="1" t="s">
         <v>30</v>
       </c>
@@ -2079,7 +2134,7 @@
       <c r="B14" s="4"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="40" t="s">
         <v>54</v>
       </c>
       <c r="F14" s="25" t="s">
@@ -2152,7 +2207,7 @@
       <c r="B20" s="4"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
-      <c r="E20" s="44"/>
+      <c r="E20" s="40"/>
       <c r="F20" s="16"/>
     </row>
     <row r="21" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2540,5 +2595,6 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>